<commit_message>
ALFA PEN EKLENDİ VE KDV AYarı yapıldı
</commit_message>
<xml_diff>
--- a/assets/excel/alfapen.xlsx
+++ b/assets/excel/alfapen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tahiratakancan/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46166E8-B7AB-A84D-A738-E754BBED7C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E6D963-6A22-8A4C-8C9F-25BEC7934399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="500" windowWidth="23240" windowHeight="17500" xr2:uid="{83D54368-FB6D-7A45-8853-F67F74174D8E}"/>
   </bookViews>
@@ -591,13 +591,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -627,11 +633,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780E2FF7-F0EC-2A4B-BACC-C1318A7B9BB5}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -978,7 +983,7 @@
     <col min="2" max="2" width="67" customWidth="1"/>
     <col min="3" max="3" width="28.83203125" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -994,7 +999,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1005,13 +1010,13 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2">
+        <v>36</v>
+      </c>
+      <c r="E2">
         <v>158</v>
       </c>
     </row>
@@ -1022,13 +1027,13 @@
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>6</v>
       </c>
       <c r="D3" s="2">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2">
+        <v>36</v>
+      </c>
+      <c r="E3">
         <v>218</v>
       </c>
     </row>
@@ -1039,13 +1044,13 @@
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2">
+        <v>24</v>
+      </c>
+      <c r="E4">
         <v>178</v>
       </c>
     </row>
@@ -1056,13 +1061,13 @@
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>6</v>
       </c>
       <c r="D5" s="2">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2">
+        <v>24</v>
+      </c>
+      <c r="E5">
         <v>263</v>
       </c>
     </row>
@@ -1073,13 +1078,13 @@
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>6</v>
-      </c>
-      <c r="E6" s="2">
+        <v>36</v>
+      </c>
+      <c r="E6">
         <v>187</v>
       </c>
     </row>
@@ -1090,13 +1095,13 @@
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="2">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2">
+        <v>36</v>
+      </c>
+      <c r="E7">
         <v>277</v>
       </c>
     </row>
@@ -1107,13 +1112,13 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>6</v>
       </c>
       <c r="D8" s="2">
-        <v>6</v>
-      </c>
-      <c r="E8" s="2">
+        <v>36</v>
+      </c>
+      <c r="E8">
         <v>185</v>
       </c>
     </row>
@@ -1124,13 +1129,13 @@
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" s="2">
-        <v>6</v>
-      </c>
-      <c r="E9" s="2">
+        <v>36</v>
+      </c>
+      <c r="E9">
         <v>277</v>
       </c>
     </row>
@@ -1141,13 +1146,13 @@
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>6</v>
       </c>
       <c r="D10" s="2">
-        <v>4</v>
-      </c>
-      <c r="E10" s="2">
+        <v>24</v>
+      </c>
+      <c r="E10">
         <v>241</v>
       </c>
     </row>
@@ -1158,13 +1163,13 @@
       <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>6</v>
       </c>
       <c r="D11" s="2">
-        <v>4</v>
-      </c>
-      <c r="E11" s="2">
+        <v>24</v>
+      </c>
+      <c r="E11">
         <v>360</v>
       </c>
     </row>
@@ -1175,13 +1180,13 @@
       <c r="B12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>6</v>
       </c>
       <c r="D12" s="2">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2">
+        <v>150</v>
+      </c>
+      <c r="E12">
         <v>55</v>
       </c>
     </row>
@@ -1192,13 +1197,13 @@
       <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>6</v>
       </c>
       <c r="D13" s="2">
-        <v>25</v>
-      </c>
-      <c r="E13" s="2">
+        <v>150</v>
+      </c>
+      <c r="E13">
         <v>98</v>
       </c>
     </row>
@@ -1209,13 +1214,13 @@
       <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2">
+        <v>150</v>
+      </c>
+      <c r="E14">
         <v>40</v>
       </c>
     </row>
@@ -1226,13 +1231,13 @@
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>6</v>
       </c>
       <c r="D15" s="2">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2">
+        <v>150</v>
+      </c>
+      <c r="E15">
         <v>74</v>
       </c>
     </row>
@@ -1243,13 +1248,13 @@
       <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>6</v>
       </c>
       <c r="D16" s="2">
-        <v>25</v>
-      </c>
-      <c r="E16" s="2">
+        <v>150</v>
+      </c>
+      <c r="E16">
         <v>38</v>
       </c>
     </row>
@@ -1260,13 +1265,13 @@
       <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>6</v>
       </c>
       <c r="D17" s="2">
-        <v>25</v>
-      </c>
-      <c r="E17" s="2">
+        <v>150</v>
+      </c>
+      <c r="E17">
         <v>67</v>
       </c>
     </row>
@@ -1277,13 +1282,13 @@
       <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>6</v>
       </c>
       <c r="D18" s="2">
-        <v>25</v>
-      </c>
-      <c r="E18" s="2">
+        <v>150</v>
+      </c>
+      <c r="E18">
         <v>40</v>
       </c>
     </row>
@@ -1294,13 +1299,13 @@
       <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>6</v>
       </c>
       <c r="D19" s="2">
-        <v>25</v>
-      </c>
-      <c r="E19" s="2">
+        <v>150</v>
+      </c>
+      <c r="E19">
         <v>74</v>
       </c>
     </row>
@@ -1311,13 +1316,13 @@
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>6</v>
       </c>
       <c r="D20" s="2">
-        <v>25</v>
-      </c>
-      <c r="E20" s="2">
+        <v>150</v>
+      </c>
+      <c r="E20">
         <v>36</v>
       </c>
     </row>
@@ -1328,13 +1333,13 @@
       <c r="B21" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>6</v>
       </c>
       <c r="D21" s="2">
-        <v>25</v>
-      </c>
-      <c r="E21" s="2">
+        <v>150</v>
+      </c>
+      <c r="E21">
         <v>64</v>
       </c>
     </row>
@@ -1345,13 +1350,13 @@
       <c r="B22" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>6.5</v>
       </c>
       <c r="D22" s="2">
-        <v>2</v>
-      </c>
-      <c r="E22" s="2">
+        <v>13</v>
+      </c>
+      <c r="E22">
         <v>326</v>
       </c>
     </row>
@@ -1362,13 +1367,13 @@
       <c r="B23" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>6.5</v>
       </c>
       <c r="D23" s="2">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2">
+        <v>13</v>
+      </c>
+      <c r="E23">
         <v>422</v>
       </c>
     </row>
@@ -1379,13 +1384,13 @@
       <c r="B24" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>6.5</v>
       </c>
       <c r="D24" s="2">
-        <v>4</v>
-      </c>
-      <c r="E24" s="2">
+        <v>26</v>
+      </c>
+      <c r="E24">
         <v>155</v>
       </c>
     </row>
@@ -1396,13 +1401,13 @@
       <c r="B25" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>6.5</v>
       </c>
       <c r="D25" s="2">
-        <v>4</v>
-      </c>
-      <c r="E25" s="2">
+        <v>26</v>
+      </c>
+      <c r="E25">
         <v>248</v>
       </c>
     </row>
@@ -1413,13 +1418,13 @@
       <c r="B26" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>6.5</v>
       </c>
       <c r="D26" s="2">
-        <v>4</v>
-      </c>
-      <c r="E26" s="2">
+        <v>26</v>
+      </c>
+      <c r="E26">
         <v>193</v>
       </c>
     </row>
@@ -1430,13 +1435,13 @@
       <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>6.5</v>
       </c>
       <c r="D27" s="2">
-        <v>4</v>
-      </c>
-      <c r="E27" s="2">
+        <v>26</v>
+      </c>
+      <c r="E27">
         <v>303</v>
       </c>
     </row>
@@ -1447,13 +1452,13 @@
       <c r="B28" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>6.5</v>
       </c>
       <c r="D28" s="2">
-        <v>4</v>
-      </c>
-      <c r="E28" s="2">
+        <v>26</v>
+      </c>
+      <c r="E28">
         <v>200</v>
       </c>
     </row>
@@ -1464,13 +1469,13 @@
       <c r="B29" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>6.5</v>
       </c>
       <c r="D29" s="2">
-        <v>4</v>
-      </c>
-      <c r="E29" s="2">
+        <v>26</v>
+      </c>
+      <c r="E29">
         <v>278</v>
       </c>
     </row>
@@ -1481,13 +1486,13 @@
       <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>6</v>
       </c>
       <c r="D30" s="2">
-        <v>4</v>
-      </c>
-      <c r="E30" s="2">
+        <v>24</v>
+      </c>
+      <c r="E30">
         <v>208</v>
       </c>
     </row>
@@ -1498,13 +1503,13 @@
       <c r="B31" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>6</v>
       </c>
       <c r="D31" s="2">
-        <v>4</v>
-      </c>
-      <c r="E31" s="2">
+        <v>24</v>
+      </c>
+      <c r="E31">
         <v>298</v>
       </c>
     </row>
@@ -1515,13 +1520,13 @@
       <c r="B32" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32">
         <v>6</v>
       </c>
       <c r="D32" s="2">
-        <v>6</v>
-      </c>
-      <c r="E32" s="2">
+        <v>36</v>
+      </c>
+      <c r="E32">
         <v>155</v>
       </c>
     </row>
@@ -1532,13 +1537,13 @@
       <c r="B33" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33">
         <v>6</v>
       </c>
       <c r="D33" s="2">
-        <v>6</v>
-      </c>
-      <c r="E33" s="2">
+        <v>36</v>
+      </c>
+      <c r="E33">
         <v>233</v>
       </c>
     </row>
@@ -1549,13 +1554,13 @@
       <c r="B34" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34">
         <v>6.5</v>
       </c>
       <c r="D34" s="2">
-        <v>4</v>
-      </c>
-      <c r="E34" s="2">
+        <v>26</v>
+      </c>
+      <c r="E34">
         <v>178</v>
       </c>
     </row>
@@ -1566,13 +1571,13 @@
       <c r="B35" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35">
         <v>6.5</v>
       </c>
       <c r="D35" s="2">
-        <v>4</v>
-      </c>
-      <c r="E35" s="2">
+        <v>26</v>
+      </c>
+      <c r="E35">
         <v>281</v>
       </c>
     </row>
@@ -1583,13 +1588,13 @@
       <c r="B36" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36">
         <v>6</v>
       </c>
       <c r="D36" s="2">
-        <v>10</v>
-      </c>
-      <c r="E36" s="2">
+        <v>60</v>
+      </c>
+      <c r="E36">
         <v>60</v>
       </c>
     </row>
@@ -1600,13 +1605,13 @@
       <c r="B37" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37">
         <v>6</v>
       </c>
       <c r="D37" s="2">
-        <v>10</v>
-      </c>
-      <c r="E37" s="2">
+        <v>60</v>
+      </c>
+      <c r="E37">
         <v>87</v>
       </c>
     </row>
@@ -1617,13 +1622,13 @@
       <c r="B38" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38">
         <v>6</v>
       </c>
       <c r="D38" s="2">
-        <v>10</v>
-      </c>
-      <c r="E38" s="2">
+        <v>60</v>
+      </c>
+      <c r="E38">
         <v>84</v>
       </c>
     </row>
@@ -1634,13 +1639,13 @@
       <c r="B39" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39">
         <v>6</v>
       </c>
       <c r="D39" s="2">
-        <v>10</v>
-      </c>
-      <c r="E39" s="2">
+        <v>60</v>
+      </c>
+      <c r="E39">
         <v>124</v>
       </c>
     </row>
@@ -1651,13 +1656,13 @@
       <c r="B40" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40">
         <v>6</v>
       </c>
       <c r="D40" s="2">
-        <v>10</v>
-      </c>
-      <c r="E40" s="2">
+        <v>60</v>
+      </c>
+      <c r="E40">
         <v>45</v>
       </c>
     </row>
@@ -1668,13 +1673,13 @@
       <c r="B41" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41">
         <v>6</v>
       </c>
       <c r="D41" s="2">
-        <v>10</v>
-      </c>
-      <c r="E41" s="2">
+        <v>60</v>
+      </c>
+      <c r="E41">
         <v>101</v>
       </c>
     </row>
@@ -1685,13 +1690,13 @@
       <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42">
         <v>6</v>
       </c>
       <c r="D42" s="2">
-        <v>25</v>
-      </c>
-      <c r="E42" s="2">
+        <v>150</v>
+      </c>
+      <c r="E42">
         <v>40</v>
       </c>
     </row>
@@ -1702,13 +1707,13 @@
       <c r="B43" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43">
         <v>6</v>
       </c>
       <c r="D43" s="2">
-        <v>25</v>
-      </c>
-      <c r="E43" s="2">
+        <v>150</v>
+      </c>
+      <c r="E43">
         <v>74</v>
       </c>
     </row>
@@ -1719,13 +1724,13 @@
       <c r="B44" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44">
         <v>6</v>
       </c>
       <c r="D44" s="2">
-        <v>25</v>
-      </c>
-      <c r="E44" s="2">
+        <v>150</v>
+      </c>
+      <c r="E44">
         <v>32</v>
       </c>
     </row>
@@ -1736,13 +1741,13 @@
       <c r="B45" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45">
         <v>6</v>
       </c>
       <c r="D45" s="2">
-        <v>25</v>
-      </c>
-      <c r="E45" s="2">
+        <v>150</v>
+      </c>
+      <c r="E45">
         <v>54</v>
       </c>
     </row>
@@ -1753,13 +1758,13 @@
       <c r="B46" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46">
         <v>6</v>
       </c>
       <c r="D46" s="2">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2">
+        <v>6</v>
+      </c>
+      <c r="E46">
         <v>590</v>
       </c>
     </row>
@@ -1770,13 +1775,13 @@
       <c r="B47" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47">
         <v>6</v>
       </c>
       <c r="D47" s="2">
-        <v>1</v>
-      </c>
-      <c r="E47" s="2">
+        <v>6</v>
+      </c>
+      <c r="E47">
         <v>590</v>
       </c>
     </row>
@@ -1787,13 +1792,13 @@
       <c r="B48" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48">
         <v>6</v>
       </c>
       <c r="D48" s="2">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2">
+        <v>6</v>
+      </c>
+      <c r="E48">
         <v>127</v>
       </c>
     </row>
@@ -1804,13 +1809,13 @@
       <c r="B49" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49">
         <v>6</v>
       </c>
       <c r="D49" s="2">
-        <v>6</v>
-      </c>
-      <c r="E49" s="2">
+        <v>36</v>
+      </c>
+      <c r="E49">
         <v>175</v>
       </c>
     </row>
@@ -1821,13 +1826,13 @@
       <c r="B50" t="s">
         <v>141</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50">
         <v>6</v>
       </c>
       <c r="D50" s="2">
-        <v>6</v>
-      </c>
-      <c r="E50" s="2">
+        <v>36</v>
+      </c>
+      <c r="E50">
         <v>240</v>
       </c>
     </row>
@@ -1838,13 +1843,13 @@
       <c r="B51" t="s">
         <v>142</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51">
         <v>6</v>
       </c>
       <c r="D51" s="2">
-        <v>4</v>
-      </c>
-      <c r="E51" s="2">
+        <v>24</v>
+      </c>
+      <c r="E51">
         <v>180</v>
       </c>
     </row>
@@ -1855,13 +1860,13 @@
       <c r="B52" t="s">
         <v>143</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52">
         <v>6</v>
       </c>
       <c r="D52" s="2">
-        <v>4</v>
-      </c>
-      <c r="E52" s="2">
+        <v>24</v>
+      </c>
+      <c r="E52">
         <v>320</v>
       </c>
     </row>
@@ -1872,13 +1877,13 @@
       <c r="B53" t="s">
         <v>145</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53">
         <v>6</v>
       </c>
       <c r="D53" s="2">
-        <v>4</v>
-      </c>
-      <c r="E53" s="2">
+        <v>24</v>
+      </c>
+      <c r="E53">
         <v>150</v>
       </c>
     </row>
@@ -1889,13 +1894,13 @@
       <c r="B54" t="s">
         <v>146</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54">
         <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>4</v>
-      </c>
-      <c r="E54" s="2">
+        <v>24</v>
+      </c>
+      <c r="E54">
         <v>263</v>
       </c>
     </row>
@@ -1906,13 +1911,13 @@
       <c r="B55" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55">
         <v>6</v>
       </c>
       <c r="D55" s="2">
-        <v>10</v>
-      </c>
-      <c r="E55" s="2">
+        <v>60</v>
+      </c>
+      <c r="E55">
         <v>143</v>
       </c>
     </row>
@@ -1923,13 +1928,13 @@
       <c r="B56" t="s">
         <v>148</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56">
         <v>6</v>
       </c>
       <c r="D56" s="2">
-        <v>10</v>
-      </c>
-      <c r="E56" s="2">
+        <v>60</v>
+      </c>
+      <c r="E56">
         <v>182</v>
       </c>
     </row>
@@ -1940,13 +1945,13 @@
       <c r="B57" t="s">
         <v>147</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57">
         <v>6</v>
       </c>
       <c r="D57" s="2">
-        <v>10</v>
-      </c>
-      <c r="E57" s="2">
+        <v>60</v>
+      </c>
+      <c r="E57">
         <v>57</v>
       </c>
     </row>
@@ -1957,13 +1962,13 @@
       <c r="B58" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58">
         <v>6</v>
       </c>
       <c r="D58" s="2">
-        <v>10</v>
-      </c>
-      <c r="E58" s="2">
+        <v>60</v>
+      </c>
+      <c r="E58">
         <v>80</v>
       </c>
     </row>
@@ -1974,13 +1979,13 @@
       <c r="B59" t="s">
         <v>150</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" s="2">
         <v>1</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59">
         <v>59</v>
       </c>
     </row>
@@ -1991,13 +1996,13 @@
       <c r="B60" t="s">
         <v>151</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" s="2">
         <v>1</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60">
         <v>59</v>
       </c>
     </row>
@@ -2008,13 +2013,13 @@
       <c r="B61" t="s">
         <v>152</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61">
         <v>6</v>
       </c>
       <c r="D61" s="2">
-        <v>6</v>
-      </c>
-      <c r="E61" s="2">
+        <v>36</v>
+      </c>
+      <c r="E61">
         <v>174</v>
       </c>
     </row>
@@ -2025,13 +2030,13 @@
       <c r="B62" t="s">
         <v>153</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62">
         <v>6</v>
       </c>
       <c r="D62" s="2">
-        <v>6</v>
-      </c>
-      <c r="E62" s="2">
+        <v>36</v>
+      </c>
+      <c r="E62">
         <v>241</v>
       </c>
     </row>
@@ -2042,13 +2047,13 @@
       <c r="B63" t="s">
         <v>154</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63">
         <v>6</v>
       </c>
       <c r="D63" s="2">
-        <v>4</v>
-      </c>
-      <c r="E63" s="2">
+        <v>24</v>
+      </c>
+      <c r="E63">
         <v>185</v>
       </c>
     </row>
@@ -2059,13 +2064,13 @@
       <c r="B64" t="s">
         <v>156</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64">
         <v>6</v>
       </c>
       <c r="D64" s="2">
-        <v>4</v>
-      </c>
-      <c r="E64" s="2">
+        <v>24</v>
+      </c>
+      <c r="E64">
         <v>323</v>
       </c>
     </row>
@@ -2076,13 +2081,13 @@
       <c r="B65" t="s">
         <v>155</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65">
         <v>6</v>
       </c>
       <c r="D65" s="2">
-        <v>8</v>
-      </c>
-      <c r="E65" s="2">
+        <v>48</v>
+      </c>
+      <c r="E65">
         <v>182</v>
       </c>
     </row>
@@ -2093,13 +2098,13 @@
       <c r="B66" t="s">
         <v>157</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66">
         <v>6</v>
       </c>
       <c r="D66" s="2">
-        <v>8</v>
-      </c>
-      <c r="E66" s="2">
+        <v>48</v>
+      </c>
+      <c r="E66">
         <v>217</v>
       </c>
     </row>
@@ -2110,13 +2115,13 @@
       <c r="B67" t="s">
         <v>158</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" s="2">
         <v>1</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67">
         <v>59</v>
       </c>
     </row>
@@ -2127,13 +2132,13 @@
       <c r="B68" t="s">
         <v>159</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68">
         <v>1</v>
       </c>
       <c r="D68" s="2">
         <v>1</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68">
         <v>59</v>
       </c>
     </row>
@@ -2144,13 +2149,13 @@
       <c r="B69" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69">
         <v>6</v>
       </c>
       <c r="D69" s="2">
-        <v>5</v>
-      </c>
-      <c r="E69" s="2">
+        <v>30</v>
+      </c>
+      <c r="E69">
         <v>151</v>
       </c>
     </row>
@@ -2161,13 +2166,13 @@
       <c r="B70" t="s">
         <v>161</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70">
         <v>6</v>
       </c>
       <c r="D70" s="2">
-        <v>5</v>
-      </c>
-      <c r="E70" s="2">
+        <v>30</v>
+      </c>
+      <c r="E70">
         <v>213</v>
       </c>
     </row>
@@ -2178,13 +2183,13 @@
       <c r="B71" t="s">
         <v>162</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71">
         <v>6</v>
       </c>
       <c r="D71" s="2">
-        <v>5</v>
-      </c>
-      <c r="E71" s="2">
+        <v>30</v>
+      </c>
+      <c r="E71">
         <v>278</v>
       </c>
     </row>
@@ -2195,13 +2200,13 @@
       <c r="B72" t="s">
         <v>163</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72">
         <v>6</v>
       </c>
       <c r="D72" s="2">
-        <v>7</v>
-      </c>
-      <c r="E72" s="2">
+        <v>42</v>
+      </c>
+      <c r="E72">
         <v>78</v>
       </c>
     </row>
@@ -2212,13 +2217,13 @@
       <c r="B73" t="s">
         <v>164</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73">
         <v>6</v>
       </c>
       <c r="D73" s="2">
-        <v>7</v>
-      </c>
-      <c r="E73" s="2">
+        <v>42</v>
+      </c>
+      <c r="E73">
         <v>194</v>
       </c>
     </row>
@@ -2229,13 +2234,13 @@
       <c r="B74" t="s">
         <v>165</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74">
         <v>6</v>
       </c>
       <c r="D74" s="2">
-        <v>7</v>
-      </c>
-      <c r="E74" s="2">
+        <v>42</v>
+      </c>
+      <c r="E74">
         <v>86</v>
       </c>
     </row>
@@ -2246,13 +2251,13 @@
       <c r="B75" t="s">
         <v>166</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75">
         <v>6</v>
       </c>
       <c r="D75" s="2">
-        <v>7</v>
-      </c>
-      <c r="E75" s="2">
+        <v>42</v>
+      </c>
+      <c r="E75">
         <v>228</v>
       </c>
     </row>
@@ -2263,13 +2268,13 @@
       <c r="B76" t="s">
         <v>167</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76">
         <v>6</v>
       </c>
       <c r="D76" s="2">
-        <v>7</v>
-      </c>
-      <c r="E76" s="2">
+        <v>42</v>
+      </c>
+      <c r="E76">
         <v>109</v>
       </c>
     </row>
@@ -2280,13 +2285,13 @@
       <c r="B77" t="s">
         <v>168</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77">
         <v>6</v>
       </c>
       <c r="D77" s="2">
-        <v>7</v>
-      </c>
-      <c r="E77" s="2">
+        <v>42</v>
+      </c>
+      <c r="E77">
         <v>302</v>
       </c>
     </row>
@@ -2297,13 +2302,13 @@
       <c r="B78" t="s">
         <v>169</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78">
         <v>6</v>
       </c>
       <c r="D78" s="2">
-        <v>10</v>
-      </c>
-      <c r="E78" s="2">
+        <v>60</v>
+      </c>
+      <c r="E78">
         <v>87</v>
       </c>
     </row>
@@ -2314,13 +2319,13 @@
       <c r="B79" t="s">
         <v>170</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79">
         <v>6</v>
       </c>
       <c r="D79" s="2">
-        <v>10</v>
-      </c>
-      <c r="E79" s="2">
+        <v>60</v>
+      </c>
+      <c r="E79">
         <v>178</v>
       </c>
     </row>
@@ -2331,13 +2336,13 @@
       <c r="B80" t="s">
         <v>171</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80">
         <v>6</v>
       </c>
       <c r="D80" s="2">
-        <v>10</v>
-      </c>
-      <c r="E80" s="2">
+        <v>60</v>
+      </c>
+      <c r="E80">
         <v>137</v>
       </c>
     </row>
@@ -2348,13 +2353,13 @@
       <c r="B81" t="s">
         <v>172</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81">
         <v>6</v>
       </c>
       <c r="D81" s="2">
-        <v>10</v>
-      </c>
-      <c r="E81" s="2">
+        <v>60</v>
+      </c>
+      <c r="E81">
         <v>221</v>
       </c>
     </row>
@@ -2365,13 +2370,13 @@
       <c r="B82" t="s">
         <v>173</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82">
         <v>6</v>
       </c>
       <c r="D82" s="2">
-        <v>25</v>
-      </c>
-      <c r="E82" s="2">
+        <v>150</v>
+      </c>
+      <c r="E82">
         <v>40</v>
       </c>
     </row>
@@ -2382,13 +2387,13 @@
       <c r="B83" t="s">
         <v>174</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83">
         <v>6</v>
       </c>
       <c r="D83" s="2">
-        <v>25</v>
-      </c>
-      <c r="E83" s="2">
+        <v>150</v>
+      </c>
+      <c r="E83">
         <v>81</v>
       </c>
     </row>
@@ -2399,13 +2404,13 @@
       <c r="B84" t="s">
         <v>175</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84">
         <v>6</v>
       </c>
       <c r="D84" s="2">
-        <v>25</v>
-      </c>
-      <c r="E84" s="2">
+        <v>150</v>
+      </c>
+      <c r="E84">
         <v>42</v>
       </c>
     </row>
@@ -2416,13 +2421,13 @@
       <c r="B85" t="s">
         <v>176</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85">
         <v>6</v>
       </c>
       <c r="D85" s="2">
-        <v>25</v>
-      </c>
-      <c r="E85" s="2">
+        <v>150</v>
+      </c>
+      <c r="E85">
         <v>80</v>
       </c>
     </row>
@@ -2433,13 +2438,13 @@
       <c r="B86" t="s">
         <v>177</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86">
         <v>6</v>
       </c>
       <c r="D86" s="2">
-        <v>20</v>
-      </c>
-      <c r="E86" s="2">
+        <v>120</v>
+      </c>
+      <c r="E86">
         <v>23</v>
       </c>
     </row>
@@ -2450,13 +2455,13 @@
       <c r="B87" t="s">
         <v>178</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87">
         <v>6</v>
       </c>
       <c r="D87" s="2">
-        <v>20</v>
-      </c>
-      <c r="E87" s="2">
+        <v>120</v>
+      </c>
+      <c r="E87">
         <v>54</v>
       </c>
     </row>
@@ -2467,13 +2472,13 @@
       <c r="B88" t="s">
         <v>179</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88">
         <v>1</v>
       </c>
       <c r="D88" s="2">
         <v>1</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88">
         <v>30</v>
       </c>
     </row>
@@ -2484,13 +2489,13 @@
       <c r="B89" t="s">
         <v>180</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89">
         <v>1</v>
       </c>
       <c r="D89" s="2">
         <v>1</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89">
         <v>23</v>
       </c>
     </row>
@@ -2501,13 +2506,13 @@
       <c r="B90" t="s">
         <v>181</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90">
         <v>1</v>
       </c>
       <c r="D90" s="2">
         <v>1</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90">
         <v>20</v>
       </c>
     </row>
@@ -2518,13 +2523,13 @@
       <c r="B91" t="s">
         <v>182</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" s="2">
         <v>1</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91">
         <v>17</v>
       </c>
     </row>

</xml_diff>